<commit_message>
working on world Matrix
</commit_message>
<xml_diff>
--- a/Utilities/Project Rubric.xlsx
+++ b/Utilities/Project Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Qsync\Graphics I &amp; II Shared Staff Folder\Project &amp; Portfolio IV\Week_3_Handout\Assignments\The Level Renderer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drave\Desktop\3dGraphics_Project\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C2B1F7-3385-405B-9FB5-6081E9791C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48999EB3-EBA6-45A7-B81B-CF588E3040C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="195" windowWidth="25335" windowHeight="16785" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">All levels must contain no less than </t>
         </r>
@@ -139,7 +139,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> unique models and at least </t>
         </r>
@@ -158,7 +158,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> duplicates of some of those models.</t>
         </r>
@@ -171,7 +171,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Exported Level Data must contain clear changes to translation, rotation and scaling of multiple models.</t>
         </r>
@@ -184,7 +184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Text Parsing must be generic and not hardcoded to a specific GameLevel's order. 
 </t>
@@ -204,7 +204,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Loop using getline('\n') to read the file till you hit the end. Whenever you find the word "MESH", the next line is the name of the model. Then use functions like atof() or sscanf() to grab the matrix data.</t>
         </r>
@@ -253,7 +253,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>No geometric glitches may be present. Must appear the same as the original. (disabling API back-face culling is allowed)</t>
         </r>
@@ -279,7 +279,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>No geometric glitches may be present. Must appear the same as the original. (disabling API back-face culling is allowed)</t>
         </r>
@@ -292,7 +292,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>There must be a variety of color and specular attributes. Textures are not required for core feature set.</t>
         </r>
@@ -305,7 +305,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Same lighting enviroment as assignment 2 at a minimum. Model materials must be utilized. Point and Spot lights also qualify but must have clear specular and ambient properties.</t>
         </r>
@@ -318,7 +318,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Unlike Core Features, you can achieve </t>
         </r>
@@ -337,7 +337,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> of these in </t>
         </r>
@@ -1263,7 +1263,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>(optional) have the python exporter script read a Blender custom attribute to get the song/FX name.</t>
         </r>
@@ -1276,7 +1276,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Provide a screenshot of your commit logs during turn-in. Additionally please add GX2Overlord as a contributor if using GitHub.</t>
         </r>
@@ -1289,7 +1289,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attatch a video clip of each in the feedback section of the Level Renderer. Include the source code/exes with this submission.</t>
         </r>
@@ -1300,7 +1300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1447,13 +1447,16 @@
   </si>
   <si>
     <t>KEY FEATURES - 33% [unlocked by core, pick three]</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1504,12 +1507,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1740,7 +1737,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
@@ -1766,10 +1763,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2095,19 +2095,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74.7109375" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -2128,8 +2129,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -2139,8 +2143,11 @@
       <c r="C3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>32</v>
       </c>
@@ -2150,8 +2157,11 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>33</v>
       </c>
@@ -2161,8 +2171,11 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2172,8 +2185,11 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2183,8 +2199,11 @@
       <c r="C7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -2195,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -2206,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2216,8 +2235,11 @@
       <c r="C10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -2227,8 +2249,11 @@
       <c r="C11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2241,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2252,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -2263,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>37</v>
       </c>
@@ -2274,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Key Features and controls done
</commit_message>
<xml_diff>
--- a/Utilities/Project Rubric.xlsx
+++ b/Utilities/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drave\Desktop\3dGraphics_Project\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE023FE-13D8-4C2D-B9DD-6EDCA104197B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37A6AB3-8C1E-48D7-B488-80ECAEB67FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1300,7 +1300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1453,9 +1453,6 @@
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
   <si>
     <t>Core</t>
@@ -2121,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2130,7 @@
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2144,7 +2141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2155,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -2172,7 +2169,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>32</v>
       </c>
@@ -2186,7 +2183,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>33</v>
       </c>
@@ -2200,7 +2197,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2214,7 +2211,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2228,7 +2225,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -2242,7 +2239,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -2256,7 +2253,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2270,7 +2267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -2284,7 +2281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2297,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2308,7 +2305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -2318,11 +2315,8 @@
       <c r="C14" s="3">
         <v>0</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>37</v>
       </c>
@@ -2332,11 +2326,8 @@
       <c r="C15" s="3">
         <v>0</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
@@ -2375,7 +2366,7 @@
         <v>50</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2392,10 +2383,10 @@
         <v>49</v>
       </c>
       <c r="G19" s="23">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2412,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2429,7 +2420,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2442,15 +2433,15 @@
       <c r="C22" s="3">
         <v>0</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>50</v>
+      <c r="D22" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="G22" s="23">
         <f>SUM(G18:G21)</f>
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2474,9 +2465,6 @@
       <c r="C24" s="3">
         <v>0</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
@@ -2738,9 +2726,6 @@
       </c>
       <c r="D46" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>